<commit_message>
info on metadata xls
</commit_message>
<xml_diff>
--- a/assets/baseMetadata.xlsx
+++ b/assets/baseMetadata.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tmnj\dev\nsi\shape-sql-loader\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8585E8CF-921C-4D04-AA7A-E5D9641E1DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD28E0F-5EF3-4BA9-A5A1-9CBF29B347F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2016" yWindow="2316" windowWidth="19044" windowHeight="8880" activeTab="4" xr2:uid="{88FD44AD-590D-43C7-9346-2FB6D77B4EB5}"/>
+    <workbookView xWindow="2220" yWindow="2196" windowWidth="19044" windowHeight="9024" activeTab="2" xr2:uid="{88FD44AD-590D-43C7-9346-2FB6D77B4EB5}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="5" r:id="rId1"/>
     <sheet name="schema" sheetId="1" r:id="rId2"/>
-    <sheet name="fields" sheetId="2" r:id="rId3"/>
+    <sheet name="fielddomain" sheetId="2" r:id="rId3"/>
     <sheet name="dataset" sheetId="3" r:id="rId4"/>
     <sheet name="access" sheetId="4" r:id="rId5"/>
   </sheets>
@@ -37,35 +37,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>testSchema</t>
-  </si>
-  <si>
     <t>version</t>
   </si>
   <si>
-    <t>0.0.1</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
-    <t>For testing only</t>
-  </si>
-  <si>
     <t>isDomain</t>
   </si>
   <si>
     <t>description</t>
   </si>
   <si>
-    <t>0.0.2</t>
-  </si>
-  <si>
     <t>purpose</t>
   </si>
   <si>
@@ -78,14 +66,86 @@
     <t>DON'T TOUCH CELLS WITH RED FONT!</t>
   </si>
   <si>
-    <t>exampleDataset</t>
+    <t>fielddomain</t>
+  </si>
+  <si>
+    <t>field description</t>
+  </si>
+  <si>
+    <t>schema</t>
+  </si>
+  <si>
+    <t>dataset</t>
+  </si>
+  <si>
+    <t>access</t>
+  </si>
+  <si>
+    <t>dataset description</t>
+  </si>
+  <si>
+    <t>dataset purpose</t>
+  </si>
+  <si>
+    <t>dataset source</t>
+  </si>
+  <si>
+    <t>dataset name</t>
+  </si>
+  <si>
+    <t>dataset version</t>
+  </si>
+  <si>
+    <t>schema name</t>
+  </si>
+  <si>
+    <t>schema version</t>
+  </si>
+  <si>
+    <t>schema desciption</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>permission</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>dataset quality - high/medium/low</t>
+  </si>
+  <si>
+    <t>field name - populated from the PreUpload CLI process</t>
+  </si>
+  <si>
+    <t>field is referenced in domain table - true if the variable is discrete categorical, false otherwise ie. including if the variable is continuous quantitative</t>
+  </si>
+  <si>
+    <t>access permission - read/add/edit/delete/all</t>
+  </si>
+  <si>
+    <t>access role - user/owner/admin</t>
+  </si>
+  <si>
+    <t>access group name</t>
+  </si>
+  <si>
+    <t>datatype</t>
+  </si>
+  <si>
+    <t>domain datatype - str/int/float</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +157,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -122,9 +190,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,10 +508,194 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A024AF0-8946-4711-97C3-05CB094F3656}">
-  <dimension ref="B1"/>
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A014777-A124-48BA-86E1-113E75DEE11B}">
+  <dimension ref="B1:B3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,47 +705,17 @@
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A014777-A124-48BA-86E1-113E75DEE11B}">
-  <dimension ref="B1:C3"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="2.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -505,7 +728,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D57ED3-1124-4C88-AE59-091C5E99248F}">
   <dimension ref="B1:D1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -517,23 +742,24 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEC2D66-2745-41D5-AB2A-E617D514554B}">
-  <dimension ref="B1:C6"/>
+  <dimension ref="B1:B6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,40 +768,34 @@
     <col min="2" max="2" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -585,15 +805,34 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F529CAD4-9FED-4DDC-9701-EF22A1A52114}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:B3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rn sheet name from fields to field-domain
</commit_message>
<xml_diff>
--- a/assets/baseMetadata.xlsx
+++ b/assets/baseMetadata.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tmnj\dev\nsi\shape-sql-loader\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4648FC85-BC7A-4C9C-B13E-B4E5EC35466E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7C8972-0D76-4859-BE39-58EC2C66D9E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2568" yWindow="2544" windowWidth="19044" windowHeight="8880" xr2:uid="{88FD44AD-590D-43C7-9346-2FB6D77B4EB5}"/>
+    <workbookView xWindow="2364" yWindow="1248" windowWidth="19044" windowHeight="8880" activeTab="2" xr2:uid="{88FD44AD-590D-43C7-9346-2FB6D77B4EB5}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="5" r:id="rId1"/>
     <sheet name="schema" sheetId="1" r:id="rId2"/>
-    <sheet name="fielddomain" sheetId="2" r:id="rId3"/>
+    <sheet name="field-domain" sheetId="2" r:id="rId3"/>
     <sheet name="dataset" sheetId="3" r:id="rId4"/>
     <sheet name="access" sheetId="4" r:id="rId5"/>
     <sheet name="quality" sheetId="6" r:id="rId6"/>
@@ -537,7 +537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A024AF0-8946-4711-97C3-05CB094F3656}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D57ED3-1124-4C88-AE59-091C5E99248F}">
   <dimension ref="B1:D1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
changed shp test source + meta xls formatting
</commit_message>
<xml_diff>
--- a/assets/baseMetadata.xlsx
+++ b/assets/baseMetadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tmnj\dev\nsi\shape-sql-loader\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5228146C-7A80-4DF8-AD33-423B7B4E30F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A194F731-87FD-4667-A976-0E0E0BFE91A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="1944" windowWidth="19044" windowHeight="8880" xr2:uid="{88FD44AD-590D-43C7-9346-2FB6D77B4EB5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{88FD44AD-590D-43C7-9346-2FB6D77B4EB5}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>name</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>a group can only have one role - each role tier includes all the permission of the previous role + additional</t>
+  </si>
+  <si>
+    <t>isPrivate</t>
   </si>
 </sst>
 </file>
@@ -532,7 +535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A024AF0-8946-4711-97C3-05CB094F3656}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -789,10 +792,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D57ED3-1124-4C88-AE59-091C5E99248F}">
-  <dimension ref="B1:D1"/>
+  <dimension ref="B1:E1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -800,7 +803,7 @@
     <col min="1" max="1" width="2.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -808,6 +811,9 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>